<commit_message>
Get Test Data Via Util Library
</commit_message>
<xml_diff>
--- a/Selenium_Framework/PythonDemo.xlsx
+++ b/Selenium_Framework/PythonDemo.xlsx
@@ -25,7 +25,7 @@
     <t xml:space="preserve">Name</t>
   </si>
   <si>
-    <t xml:space="preserve">Fname</t>
+    <t xml:space="preserve">FirstName</t>
   </si>
   <si>
     <t xml:space="preserve">Email</t>
@@ -179,12 +179,16 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -208,12 +212,12 @@
   <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H16" activeCellId="0" sqref="H16"/>
+      <selection pane="topLeft" activeCell="D1" activeCellId="0" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="17.8906882591093"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="17.995951417004"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="0" width="10.7125506072875"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="0" width="13.6032388663968"/>
     <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="8.57085020242915"/>
@@ -223,13 +227,13 @@
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
     </row>

</xml_diff>